<commit_message>
v0.0.11 Synthetic Data Page UI
</commit_message>
<xml_diff>
--- a/Job_Details.xlsx
+++ b/Job_Details.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="21">
   <si>
     <t>INT</t>
   </si>
@@ -67,6 +67,18 @@
   </si>
   <si>
     <t>24-04-2020 20:12:14</t>
+  </si>
+  <si>
+    <t>Trades_10m</t>
+  </si>
+  <si>
+    <t>26-04-2020 10:21:54</t>
+  </si>
+  <si>
+    <t>Transactions</t>
+  </si>
+  <si>
+    <t>26-04-2020 20:06:47</t>
   </si>
 </sst>
 </file>
@@ -406,7 +418,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -561,6 +573,82 @@
         <v>7</v>
       </c>
       <c r="L4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="B5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J5" t="s">
+        <v>6</v>
+      </c>
+      <c r="K5" t="s">
+        <v>7</v>
+      </c>
+      <c r="L5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" t="s">
+        <v>4</v>
+      </c>
+      <c r="H6" t="s">
+        <v>20</v>
+      </c>
+      <c r="I6" t="s">
+        <v>20</v>
+      </c>
+      <c r="J6" t="s">
+        <v>6</v>
+      </c>
+      <c r="K6" t="s">
+        <v>7</v>
+      </c>
+      <c r="L6" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
v0.1.1 Integrated Synthetic Java REST calls copyDB.js broken
</commit_message>
<xml_diff>
--- a/Job_Details.xlsx
+++ b/Job_Details.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="25">
   <si>
     <t>INT</t>
   </si>
@@ -85,6 +85,12 @@
   </si>
   <si>
     <t>27-04-2020 11:36:57</t>
+  </si>
+  <si>
+    <t>28-04-2020 09:36:03</t>
+  </si>
+  <si>
+    <t>28-04-2020 10:05:55</t>
   </si>
 </sst>
 </file>
@@ -424,7 +430,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -693,6 +699,82 @@
         <v>7</v>
       </c>
       <c r="L7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" t="s">
+        <v>1</v>
+      </c>
+      <c r="F8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H8" t="s">
+        <v>23</v>
+      </c>
+      <c r="I8" t="s">
+        <v>23</v>
+      </c>
+      <c r="J8" t="s">
+        <v>6</v>
+      </c>
+      <c r="K8" t="s">
+        <v>7</v>
+      </c>
+      <c r="L8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="B9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G9" t="s">
+        <v>4</v>
+      </c>
+      <c r="H9" t="s">
+        <v>24</v>
+      </c>
+      <c r="I9" t="s">
+        <v>24</v>
+      </c>
+      <c r="J9" t="s">
+        <v>6</v>
+      </c>
+      <c r="K9" t="s">
+        <v>7</v>
+      </c>
+      <c r="L9" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
v0.2.3 Reset fixed | Filter Value changed to Synthetic Value
</commit_message>
<xml_diff>
--- a/Job_Details.xlsx
+++ b/Job_Details.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="29">
   <si>
     <t>INT</t>
   </si>
@@ -91,6 +91,18 @@
   </si>
   <si>
     <t>28-04-2020 10:05:55</t>
+  </si>
+  <si>
+    <t>04-05-2020 14:25:55</t>
+  </si>
+  <si>
+    <t>04-05-2020 14:32:07</t>
+  </si>
+  <si>
+    <t>04-05-2020 14:36:45</t>
+  </si>
+  <si>
+    <t>04-05-2020 14:42:59</t>
   </si>
 </sst>
 </file>
@@ -430,7 +442,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -775,6 +787,158 @@
         <v>7</v>
       </c>
       <c r="L9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="B10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" t="s">
+        <v>0</v>
+      </c>
+      <c r="E10" t="s">
+        <v>2</v>
+      </c>
+      <c r="F10" t="s">
+        <v>15</v>
+      </c>
+      <c r="G10" t="s">
+        <v>12</v>
+      </c>
+      <c r="H10" t="s">
+        <v>25</v>
+      </c>
+      <c r="I10" t="s">
+        <v>25</v>
+      </c>
+      <c r="J10" t="s">
+        <v>6</v>
+      </c>
+      <c r="K10" t="s">
+        <v>7</v>
+      </c>
+      <c r="L10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="B11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" t="s">
+        <v>2</v>
+      </c>
+      <c r="F11" t="s">
+        <v>3</v>
+      </c>
+      <c r="G11" t="s">
+        <v>12</v>
+      </c>
+      <c r="H11" t="s">
+        <v>26</v>
+      </c>
+      <c r="I11" t="s">
+        <v>26</v>
+      </c>
+      <c r="J11" t="s">
+        <v>6</v>
+      </c>
+      <c r="K11" t="s">
+        <v>7</v>
+      </c>
+      <c r="L11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="B12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12" t="s">
+        <v>0</v>
+      </c>
+      <c r="E12" t="s">
+        <v>2</v>
+      </c>
+      <c r="F12" t="s">
+        <v>3</v>
+      </c>
+      <c r="G12" t="s">
+        <v>4</v>
+      </c>
+      <c r="H12" t="s">
+        <v>27</v>
+      </c>
+      <c r="I12" t="s">
+        <v>27</v>
+      </c>
+      <c r="J12" t="s">
+        <v>6</v>
+      </c>
+      <c r="K12" t="s">
+        <v>7</v>
+      </c>
+      <c r="L12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="B13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" t="s">
+        <v>0</v>
+      </c>
+      <c r="E13" t="s">
+        <v>1</v>
+      </c>
+      <c r="F13" t="s">
+        <v>3</v>
+      </c>
+      <c r="G13" t="s">
+        <v>4</v>
+      </c>
+      <c r="H13" t="s">
+        <v>28</v>
+      </c>
+      <c r="I13" t="s">
+        <v>28</v>
+      </c>
+      <c r="J13" t="s">
+        <v>6</v>
+      </c>
+      <c r="K13" t="s">
+        <v>7</v>
+      </c>
+      <c r="L13" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
v0.3.0 jar changed to war jsp and static folders moved
</commit_message>
<xml_diff>
--- a/Job_Details.xlsx
+++ b/Job_Details.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="34">
   <si>
     <t>INT</t>
   </si>
@@ -103,6 +103,21 @@
   </si>
   <si>
     <t>04-05-2020 14:42:59</t>
+  </si>
+  <si>
+    <t>UAT12</t>
+  </si>
+  <si>
+    <t>RRD</t>
+  </si>
+  <si>
+    <t>PROD18</t>
+  </si>
+  <si>
+    <t>JRD</t>
+  </si>
+  <si>
+    <t>10-05-2020 22:29:18</t>
   </si>
 </sst>
 </file>
@@ -442,7 +457,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L13"/>
+  <dimension ref="A1:L14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -939,6 +954,44 @@
         <v>7</v>
       </c>
       <c r="L13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>13.0</v>
+      </c>
+      <c r="B14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" t="s">
+        <v>31</v>
+      </c>
+      <c r="E14" t="s">
+        <v>32</v>
+      </c>
+      <c r="F14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14" t="s">
+        <v>4</v>
+      </c>
+      <c r="H14" t="s">
+        <v>33</v>
+      </c>
+      <c r="I14" t="s">
+        <v>33</v>
+      </c>
+      <c r="J14" t="s">
+        <v>6</v>
+      </c>
+      <c r="K14" t="s">
+        <v>7</v>
+      </c>
+      <c r="L14" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>